<commit_message>
feat: add comprehensive notification system with floating widget
- Add system tray integration with context menu controls
- Implement floating status widget for real-time execution monitoring
- Add preparation widget for workflow setup and verification
- Enhance progress calculation with step-level tracking
- Add execution preparation phase with checklist
- Improve OCR text extraction with better error handling
- Update hotkey listener for better system tray integration
- Add comprehensive E2E tests for notification features
- Fix various workflow execution bugs and edge cases
- Update CLAUDE.md with MCP installation guidelines

This update significantly improves user experience by providing
visual feedback during macro execution and allowing background
operation through system tray integration.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/demo_data.xlsx
+++ b/demo_data.xlsx
@@ -466,10 +466,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>001</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -493,15 +491,13 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>대기</t>
+          <t>실패: Step '텍스트 검색' failed: TextExtractor.find_text() got an unexpected keyword argument 'confidence'</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -525,15 +521,13 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>대기</t>
+          <t>실패: Step '텍스트 검색' failed: TextExtractor.find_text() got an unexpected keyword argument 'confidence'</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>003</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -557,15 +551,13 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>대기</t>
+          <t>실패: Step '텍스트 검색' failed: TextExtractor.find_text() got an unexpected keyword argument 'confidence'</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>004</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -589,15 +581,13 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>대기</t>
+          <t>실패: Step '텍스트 검색' failed: TextExtractor.find_text() got an unexpected keyword argument 'confidence'</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>005</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -621,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>대기</t>
+          <t>실패: Step '텍스트 검색' failed: TextExtractor.find_text() got an unexpected keyword argument 'confidence'</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: analyze text search functionality issues and prepare for fixes
- Comprehensive analysis of text search feature implementation
- Identified variable substitution inconsistencies between dialog and executor
- Found region data preservation issues in step configuration
- Documented OCR initialization and error handling problems
- Analyzed performance bottlenecks in text extraction
- Prepared detailed solution plan for fixing intermittent failures
</commit_message>
<xml_diff>
--- a/demo_data.xlsx
+++ b/demo_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>미완료</t>
+          <t>오류</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -533,7 +533,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>미완료</t>
+          <t>오류</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>미완료</t>
+          <t>오류</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -597,7 +597,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>미완료</t>
+          <t>오류</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -629,7 +629,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>미완료</t>
+          <t>오류</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>

</xml_diff>